<commit_message>
TestNGRunner class added with stepDefinations and all
</commit_message>
<xml_diff>
--- a/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
+++ b/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408293\git\Team_ChatureBhature_IdentifyCourses\IdentifyCourses.Coursera.org\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35423CA-CC88-49A9-861A-230D99216CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58266DE1-1AE8-4D2C-8893-10A6DB8C4771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E2ACAEC7-E164-4C10-81D1-F69421976CEC}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,11 +36,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t>Languages And Count</t>
+  </si>
+  <si>
+    <t>Croatian(1)</t>
+  </si>
+  <si>
+    <t>Azerbaijani(477)</t>
+  </si>
+  <si>
+    <t>Dutch(2,126)</t>
+  </si>
+  <si>
+    <t>Polish(2,133)</t>
+  </si>
+  <si>
+    <t>Portuguese (Brazil)(2,389)</t>
+  </si>
+  <si>
+    <t>Chinese (China)(2,347)</t>
+  </si>
+  <si>
+    <t>Hindi(2,218)</t>
+  </si>
+  <si>
+    <t>Swedish(2,127)</t>
+  </si>
+  <si>
+    <t>Vietnamese(505)</t>
+  </si>
+  <si>
+    <t>Hebrew(6)</t>
+  </si>
+  <si>
+    <t>Kazakh(1,948)</t>
+  </si>
+  <si>
+    <t>Ukrainian(2,156)</t>
+  </si>
+  <si>
+    <t>Portuguese (Portugal)(1)</t>
+  </si>
+  <si>
+    <t>French(2,402)</t>
+  </si>
+  <si>
+    <t>Italian(2,160)</t>
+  </si>
+  <si>
+    <t>Spanish(2,669)</t>
+  </si>
+  <si>
+    <t>Chinese (Traditional)(45)</t>
+  </si>
+  <si>
+    <t>Korean(2,235)</t>
+  </si>
+  <si>
+    <t>English(5,859)</t>
+  </si>
+  <si>
+    <t>Pushto(259)</t>
+  </si>
+  <si>
+    <t>Catalan(1)</t>
+  </si>
+  <si>
+    <t>Arabic(2,403)</t>
+  </si>
+  <si>
+    <t>Uzbek(567)</t>
+  </si>
+  <si>
+    <t>Russian(2,259)</t>
+  </si>
+  <si>
+    <t>Turkish(2,177)</t>
+  </si>
+  <si>
+    <t>Indonesian(2,313)</t>
+  </si>
+  <si>
+    <t>Greek(2,127)</t>
+  </si>
+  <si>
+    <t>Thai(2,140)</t>
+  </si>
+  <si>
+    <t>German(2,331)</t>
+  </si>
+  <si>
+    <t>Hungarian(1,372)</t>
+  </si>
+  <si>
+    <t>Japanese(2,314)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -406,14 +504,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5447F97-9D47-40AC-AE8E-7981387DE99A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="A1:XFD1048576"/>
+      <selection activeCell="C5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved the errors which were encountering
</commit_message>
<xml_diff>
--- a/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
+++ b/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408293\git\Team_ChatureBhature_IdentifyCourses\IdentifyCourses.Coursera.org\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58266DE1-1AE8-4D2C-8893-10A6DB8C4771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC272BAB-A1EC-47FF-B841-8D31F9181867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E2ACAEC7-E164-4C10-81D1-F69421976CEC}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,109 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>Languages And Count</t>
-  </si>
-  <si>
-    <t>Croatian(1)</t>
-  </si>
-  <si>
-    <t>Azerbaijani(477)</t>
-  </si>
-  <si>
-    <t>Dutch(2,126)</t>
-  </si>
-  <si>
-    <t>Polish(2,133)</t>
-  </si>
-  <si>
-    <t>Portuguese (Brazil)(2,389)</t>
-  </si>
-  <si>
-    <t>Chinese (China)(2,347)</t>
-  </si>
-  <si>
-    <t>Hindi(2,218)</t>
-  </si>
-  <si>
-    <t>Swedish(2,127)</t>
-  </si>
-  <si>
-    <t>Vietnamese(505)</t>
-  </si>
-  <si>
-    <t>Hebrew(6)</t>
-  </si>
-  <si>
-    <t>Kazakh(1,948)</t>
-  </si>
-  <si>
-    <t>Ukrainian(2,156)</t>
-  </si>
-  <si>
-    <t>Portuguese (Portugal)(1)</t>
-  </si>
-  <si>
-    <t>French(2,402)</t>
-  </si>
-  <si>
-    <t>Italian(2,160)</t>
-  </si>
-  <si>
-    <t>Spanish(2,669)</t>
-  </si>
-  <si>
-    <t>Chinese (Traditional)(45)</t>
-  </si>
-  <si>
-    <t>Korean(2,235)</t>
-  </si>
-  <si>
-    <t>English(5,859)</t>
-  </si>
-  <si>
-    <t>Pushto(259)</t>
-  </si>
-  <si>
-    <t>Catalan(1)</t>
-  </si>
-  <si>
-    <t>Arabic(2,403)</t>
-  </si>
-  <si>
-    <t>Uzbek(567)</t>
-  </si>
-  <si>
-    <t>Russian(2,259)</t>
-  </si>
-  <si>
-    <t>Turkish(2,177)</t>
-  </si>
-  <si>
-    <t>Indonesian(2,313)</t>
-  </si>
-  <si>
-    <t>Greek(2,127)</t>
-  </si>
-  <si>
-    <t>Thai(2,140)</t>
-  </si>
-  <si>
-    <t>German(2,331)</t>
-  </si>
-  <si>
-    <t>Hungarian(1,372)</t>
-  </si>
-  <si>
-    <t>Japanese(2,314)</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -504,175 +406,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5447F97-9D47-40AC-AE8E-7981387DE99A}">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="0">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="0">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s" s="0">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="0">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor bug fixes and changes to the code were made after Akshats commit
</commit_message>
<xml_diff>
--- a/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
+++ b/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408293\git\Team_ChatureBhature_IdentifyCourses\IdentifyCourses.Coursera.org\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C2140-D0B9-41F0-9216-5336A6531676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBB2974-7958-49E2-810D-710CBDA6255D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E2ACAEC7-E164-4C10-81D1-F69421976CEC}"/>
   </bookViews>
@@ -167,17 +167,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,275 +503,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5447F97-9D47-40AC-AE8E-7981387DE99A}">
-  <dimension ref="A1:A65"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C13" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="2"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="2"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" s="2"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="2"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" s="2"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" s="2"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="2"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="2"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" s="2"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" s="2"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" s="2"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="2"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" s="2"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" s="2"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" s="2"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59" s="2"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" s="2"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A61" s="2"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A62" s="2"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A63" s="2"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A64" s="3"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
The Final version of the project is released
</commit_message>
<xml_diff>
--- a/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
+++ b/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408293\git\Team_ChatureBhature_IdentifyCourses\IdentifyCourses.Coursera.org\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBB2974-7958-49E2-810D-710CBDA6255D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9DCC5E-2139-4BC1-AD51-DEF9BA6ED659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E2ACAEC7-E164-4C10-81D1-F69421976CEC}"/>
   </bookViews>
@@ -36,104 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>Languages And Count</t>
-  </si>
-  <si>
-    <t>Croatian(1)</t>
-  </si>
-  <si>
-    <t>Azerbaijani(477)</t>
-  </si>
-  <si>
-    <t>Dutch(2,126)</t>
-  </si>
-  <si>
-    <t>Polish(2,133)</t>
-  </si>
-  <si>
-    <t>Portuguese (Brazil)(2,389)</t>
-  </si>
-  <si>
-    <t>Chinese (China)(2,347)</t>
-  </si>
-  <si>
-    <t>Hindi(2,218)</t>
-  </si>
-  <si>
-    <t>Swedish(2,127)</t>
-  </si>
-  <si>
-    <t>Vietnamese(505)</t>
-  </si>
-  <si>
-    <t>Hebrew(6)</t>
-  </si>
-  <si>
-    <t>Kazakh(1,948)</t>
-  </si>
-  <si>
-    <t>Ukrainian(2,156)</t>
-  </si>
-  <si>
-    <t>Portuguese (Portugal)(1)</t>
-  </si>
-  <si>
-    <t>French(2,402)</t>
-  </si>
-  <si>
-    <t>Italian(2,160)</t>
-  </si>
-  <si>
-    <t>Spanish(2,669)</t>
-  </si>
-  <si>
-    <t>Chinese (Traditional)(45)</t>
-  </si>
-  <si>
-    <t>Korean(2,235)</t>
-  </si>
-  <si>
-    <t>English(5,859)</t>
-  </si>
-  <si>
-    <t>Pushto(259)</t>
-  </si>
-  <si>
-    <t>Catalan(1)</t>
-  </si>
-  <si>
-    <t>Arabic(2,403)</t>
-  </si>
-  <si>
-    <t>Uzbek(567)</t>
-  </si>
-  <si>
-    <t>Russian(2,259)</t>
-  </si>
-  <si>
-    <t>Turkish(2,177)</t>
-  </si>
-  <si>
-    <t>Indonesian(2,313)</t>
-  </si>
-  <si>
-    <t>Greek(2,127)</t>
-  </si>
-  <si>
-    <t>Thai(2,140)</t>
-  </si>
-  <si>
-    <t>German(2,331)</t>
-  </si>
-  <si>
-    <t>Hungarian(1,372)</t>
-  </si>
-  <si>
-    <t>Japanese(2,314)</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -503,175 +406,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5447F97-9D47-40AC-AE8E-7981387DE99A}">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="A1:XFD1048576"/>
+      <selection activeCell="D14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit made by Shivendra to get updated
</commit_message>
<xml_diff>
--- a/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
+++ b/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408293\git\Team_ChatureBhature_IdentifyCourses\IdentifyCourses.Coursera.org\src\test\resources\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>Languages And Count</t>
   </si>
@@ -138,6 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5447F97-9D47-40AC-AE8E-7981387DE99A}">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:A63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="A1:XFD1048576"/>
@@ -512,162 +513,317 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" t="s" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" t="s" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" t="s" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" t="s" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="A31" t="s" s="0">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit made by Anuj to get updated
</commit_message>
<xml_diff>
--- a/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
+++ b/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408293\git\Team_ChatureBhature_IdentifyCourses\IdentifyCourses.Coursera.org\src\test\resources\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>Languages And Count</t>
   </si>
@@ -138,6 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5447F97-9D47-40AC-AE8E-7981387DE99A}">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:A63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="A1:XFD1048576"/>
@@ -512,162 +513,317 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" t="s" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" t="s" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" t="s" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" t="s" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="A31" t="s" s="0">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit by Akshat Anand
</commit_message>
<xml_diff>
--- a/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
+++ b/IdentifyCourses.Coursera.org/src/test/resources/Count_Of_Languages.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408293\git\Team_ChatureBhature_IdentifyCourses\IdentifyCourses.Coursera.org\src\test\resources\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>Languages And Count</t>
   </si>
@@ -138,6 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5447F97-9D47-40AC-AE8E-7981387DE99A}">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:A63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="A1:XFD1048576"/>
@@ -512,162 +513,317 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" t="s" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" t="s" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" t="s" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" t="s" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="A31" t="s" s="0">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
         <v>31</v>
       </c>
     </row>

</xml_diff>